<commit_message>
45 with PID of voltage
</commit_message>
<xml_diff>
--- a/working/2025最新计算器.xlsx
+++ b/working/2025最新计算器.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HRb\HydrogenRb\Work\Robomaster\2024 - 2025\2 supercap database\PurdueRMSuperCap\working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HydrogenRb\HydrogenRb\Work\Robomaster\1 SuperCap\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E81C532-BD87-448D-A677-9CCC2099AFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510FE358-F0A3-47A1-96A4-24674CC004AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1605" windowWidth="17280" windowHeight="9983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -391,15 +389,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="17.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -410,19 +408,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2311</v>
+        <v>300</v>
       </c>
       <c r="C2">
         <f>B2*(3.3/4095)*11</f>
-        <v>20.485787545787545</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.6593406593406592</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -430,16 +428,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <f>B4*4095/3.3/11</f>
-        <v>451.23966942148763</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>225.61983471074382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -453,19 +451,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9">
-        <v>3202</v>
+        <v>3300</v>
       </c>
       <c r="C9">
         <v>2047</v>
       </c>
       <c r="D9">
         <f>0.00644689*(B9-C9)</f>
-        <v>7.4461579499999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8.0779531700000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -473,13 +471,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <f>(B11+C9*0.00644689)/0.00644689</f>
-        <v>3132.7948561244261</v>
+        <v>3598.1355087491797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>